<commit_message>
Scripts and test cases updated
</commit_message>
<xml_diff>
--- a/solution/JCManual TestCases.xlsx
+++ b/solution/JCManual TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\venky\vc\JumpCloud\solution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arrowelectronics-my.sharepoint.com/personal/vchunduri_arrow_com/Documents/Documents/GitHub/JCTest/solution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3433781E-6E23-426D-A657-9E0EA82DEA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{3433781E-6E23-426D-A657-9E0EA82DEA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D4E7C2B-4BF0-4383-B026-9F64A888590D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C637035A-B07A-4C14-AC6B-117BAF9175AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C637035A-B07A-4C14-AC6B-117BAF9175AB}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="114">
   <si>
     <t>REQUIREMENT INFORMATION</t>
   </si>
@@ -320,10 +320,6 @@
 "Hash not found"</t>
   </si>
   <si>
-    <t xml:space="preserve"> below message displayed
-"Hash not found"</t>
-  </si>
-  <si>
     <t>200 OK status code on get request and a corresponding encoded password for job id is displayed</t>
   </si>
   <si>
@@ -443,6 +439,23 @@
   <si>
     <t>No password validation user can enter any password
 commented in the given info</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> below message displayed
+"Hash not found"
+expected 404 but seeing 400</t>
+  </si>
+  <si>
+    <t>Step6</t>
+  </si>
+  <si>
+    <t>Verify that request take at least 5sec to complete</t>
+  </si>
+  <si>
+    <t>From postman the request should take greater than 5Sec.</t>
+  </si>
+  <si>
+    <t>request took 5.01s</t>
   </si>
 </sst>
 </file>
@@ -596,11 +609,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -919,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE87BF3-D9E1-42B3-99B5-5705664431EC}">
   <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -932,13 +945,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
@@ -951,10 +964,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -967,7 +980,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -980,7 +993,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -993,7 +1006,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1007,10 +1020,10 @@
         <v>56</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="120" x14ac:dyDescent="0.25">
@@ -1024,10 +1037,10 @@
         <v>68</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1041,10 +1054,10 @@
         <v>69</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1057,11 +1070,11 @@
       <c r="D10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>107</v>
+      <c r="E10" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1075,10 +1088,10 @@
         <v>71</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1091,7 +1104,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1110,11 +1123,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1B08CA-226F-4DB7-AFEC-D83376410140}">
-  <dimension ref="B1:K18"/>
+  <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1174,7 @@
         <v>27</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="60" x14ac:dyDescent="0.25">
@@ -1254,12 +1267,12 @@
       </c>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>53</v>
@@ -1271,13 +1284,13 @@
         <v>48</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>37</v>
@@ -1286,25 +1299,25 @@
     </row>
     <row r="6" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>54</v>
+      <c r="D6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>49</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>47</v>
@@ -1314,37 +1327,37 @@
       </c>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="2:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>58</v>
+        <v>28</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1358,10 +1371,10 @@
         <v>59</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>60</v>
@@ -1372,41 +1385,41 @@
       <c r="J8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="K9" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1419,14 +1432,14 @@
       <c r="E10" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>33</v>
+      <c r="F10" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>75</v>
@@ -1436,7 +1449,7 @@
       </c>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="2:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1450,23 +1463,23 @@
         <v>66</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1480,108 +1493,108 @@
         <v>66</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="2:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E13" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>101</v>
+      <c r="H13" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="2:11" ht="180" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G15" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="2:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>37</v>
@@ -1593,82 +1606,112 @@
         <v>20</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="H16" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>99</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="K16" s="7"/>
     </row>
     <row r="17" spans="2:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C17" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="2:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
       <c r="C18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>90</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="11" t="s">
+      <c r="G18" s="7"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="7"/>
+      <c r="K19" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>